<commit_message>
final files after acceptance
</commit_message>
<xml_diff>
--- a/Manuscript/20230611_Re-submitted/Appendix_S3.xlsx
+++ b/Manuscript/20230611_Re-submitted/Appendix_S3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethandruszkiewicz/GoogleDrive/UW/GitHub/quantitative_salmon_resubmit/Manuscript/20230611_Re-submitted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5E12A1-D5F0-2A4E-AFD0-AAF03C038831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58604FA-2B34-CE49-B488-B0D0A293EAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="1080" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8400" yWindow="1080" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="4" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$B$16</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">TableS1!$A$1:$D$26</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">TableS2!$A$1:$F$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">TableS1!$A$3:$D$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">TableS2!$A$3:$F$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="118">
   <si>
     <t>Species</t>
   </si>
@@ -728,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -867,6 +867,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -913,17 +922,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
@@ -931,6 +934,18 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1289,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AE889A-4836-A94C-BD94-85416A3E26AE}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1380,342 +1395,351 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" thickBot="1">
+      <c r="A3" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" thickTop="1">
-      <c r="A2" s="2" t="s">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
+      <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="C26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1727,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1740,697 +1764,717 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="11"/>
+      <c r="B4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="10" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B5" s="10">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C5" s="5">
         <f>1/18</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D5" s="9">
         <v>4.48E-2</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E5" s="6">
         <v>0.05</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F5" s="5">
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="10" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B6" s="10">
         <v>9.5200000000000007E-2</v>
       </c>
-      <c r="C4" s="7">
-        <f t="shared" ref="C4:C24" si="0">1/18</f>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:C26" si="0">1/18</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D6" s="9">
         <v>4.48E-2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E6" s="6">
         <v>0.05</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F6" s="5">
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="10" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B7" s="10">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C7" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D7" s="9">
         <v>8.9700000000000002E-2</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E7" s="6">
         <v>0.05</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F7" s="5">
         <v>7.0900000000000005E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="10" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B8" s="10">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C8" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D8" s="9">
         <v>4.48E-2</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E8" s="6">
         <v>0.05</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F8" s="5">
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="10" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B9" s="10">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C9" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D9" s="9">
         <v>8.9700000000000002E-2</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E9" s="6">
         <v>0.05</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F9" s="5">
         <v>0.10639999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="10" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B10" s="10">
         <v>0.1905</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C10" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D10" s="9">
         <v>0.22420000000000001</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E10" s="6">
         <v>0.05</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F10" s="5">
         <v>0.1774</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="10" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B11" s="10">
         <v>1.9E-2</v>
       </c>
-      <c r="C9" s="8">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="10" t="s">
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B12" s="10">
         <v>1.9E-2</v>
       </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
         <v>0.05</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F12" s="5">
         <v>1.77E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="10" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B13" s="10">
         <v>7.6200000000000004E-2</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C13" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D13" s="9">
         <v>0.13450000000000001</v>
       </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="10" t="s">
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B14" s="10">
         <v>0.1905</v>
       </c>
-      <c r="C12" s="8">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
         <v>0.05</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F14" s="5">
         <v>7.0900000000000005E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="10" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B15" s="10">
         <v>8.5699999999999998E-2</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C15" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D15" s="9">
         <v>3.3599999999999998E-2</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="10" t="s">
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B16" s="10">
         <v>8.5699999999999998E-2</v>
       </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
         <v>0.05</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F16" s="5">
         <v>7.0900000000000005E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="10" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="8">
-        <v>0</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D17" s="9">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E17" s="6">
         <v>0.05</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F17" s="5">
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="10" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D18" s="9">
         <v>6.7299999999999999E-2</v>
       </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="10" t="s">
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D19" s="9">
         <v>1.7899999999999999E-2</v>
       </c>
-      <c r="E17" s="8">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="10" t="s">
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="8">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D20" s="9">
         <v>3.3599999999999998E-2</v>
       </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="10" t="s">
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D21" s="9">
         <v>1.12E-2</v>
       </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="10" t="s">
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="8">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D22" s="9">
         <v>6.7299999999999999E-2</v>
       </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="10" t="s">
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="8">
-        <v>0</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D23" s="9">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="10" t="s">
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="8">
-        <v>0</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D24" s="9">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="10" t="s">
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="8">
-        <v>0</v>
-      </c>
-      <c r="C23" s="7">
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D25" s="9">
         <v>3.3599999999999998E-2</v>
       </c>
-      <c r="E23" s="8">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="10" t="s">
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="8">
-        <v>0</v>
-      </c>
-      <c r="C24" s="7">
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D26" s="9">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E24" s="8">
-        <v>0</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="10" t="s">
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="8">
-        <v>0</v>
-      </c>
-      <c r="C25" s="8">
-        <v>0</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-      <c r="E25" s="8">
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6">
         <v>0.05</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F27" s="5">
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="10" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="8">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8">
-        <v>0</v>
-      </c>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8">
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
         <v>0.05</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F28" s="5">
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="10" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="8">
-        <v>0</v>
-      </c>
-      <c r="C27" s="8">
-        <v>0</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0</v>
-      </c>
-      <c r="E27" s="8">
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6">
         <v>0.05</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F29" s="5">
         <v>8.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="10" t="s">
+    <row r="30" spans="1:6">
+      <c r="A30" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="8">
-        <v>0</v>
-      </c>
-      <c r="C28" s="8">
-        <v>0</v>
-      </c>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-      <c r="E28" s="8">
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6">
         <v>0.05</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F30" s="5">
         <v>7.0900000000000005E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="10" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="8">
-        <v>0</v>
-      </c>
-      <c r="C29" s="8">
-        <v>0</v>
-      </c>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
-      <c r="E29" s="8">
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
         <v>0.05</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F31" s="5">
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="10" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="8">
-        <v>0</v>
-      </c>
-      <c r="C30" s="8">
-        <v>0</v>
-      </c>
-      <c r="D30" s="9">
-        <v>0</v>
-      </c>
-      <c r="E30" s="8">
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
         <v>0.05</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F32" s="5">
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="10" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="8">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8">
-        <v>0</v>
-      </c>
-      <c r="D31" s="9">
-        <v>0</v>
-      </c>
-      <c r="E31" s="8">
+      <c r="B33" s="6">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6">
         <v>0.05</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F33" s="5">
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="10" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="8">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8">
-        <v>0</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0</v>
-      </c>
-      <c r="E32" s="8">
+      <c r="B34" s="6">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
         <v>0.05</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F34" s="5">
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="10" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="8">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8">
-        <v>0</v>
-      </c>
-      <c r="D33" s="9">
-        <v>0</v>
-      </c>
-      <c r="E33" s="8">
+      <c r="B35" s="6">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0</v>
+      </c>
+      <c r="E35" s="6">
         <v>0.05</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F35" s="5">
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="10" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="8">
-        <v>0</v>
-      </c>
-      <c r="C34" s="8">
-        <v>0</v>
-      </c>
-      <c r="D34" s="9">
-        <v>0</v>
-      </c>
-      <c r="E34" s="8">
+      <c r="B36" s="6">
+        <v>0</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0</v>
+      </c>
+      <c r="E36" s="6">
         <v>0.05</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F36" s="5">
         <v>7.0900000000000005E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>